<commit_message>
Added dependencies and key for each user story in User stories classified.xlsx Some minor grammar edits as well
</commit_message>
<xml_diff>
--- a/DomainsModel/User stories classified.xlsx
+++ b/DomainsModel/User stories classified.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everybody's\Desktop\R&amp;D\R-D-AUT-Mathex-Development Branch\DomainsModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haylis\Desktop\R-D\DomainsModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="86">
   <si>
     <t>User Story</t>
   </si>
@@ -162,9 +162,6 @@
     <t>As a marker, I want to be request to confirm any of my actions so that I don’t make mistakes.</t>
   </si>
   <si>
-    <t xml:space="preserve">As a marker, I want to receive feedback from the application for all my interactions so that I know it has been successful. </t>
-  </si>
-  <si>
     <t>Admin User Stories:</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
   </si>
   <si>
     <t>As a privileged user, I want to be able to log in with a user name and password so that I can securely access my account.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be redirect to my user type properly so that I don’t have to navigate to it manually.  </t>
   </si>
   <si>
     <t>Spectator User Stories:</t>
@@ -300,6 +294,135 @@
   </si>
   <si>
     <t>As a marker, I want to be the only marker assigned to a specific team so that there is no conflict in marking.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want to be redirected to my user type properly so that I don’t have to navigate to it manually.  </t>
+  </si>
+  <si>
+    <t>US1</t>
+  </si>
+  <si>
+    <t>US2</t>
+  </si>
+  <si>
+    <t>US3</t>
+  </si>
+  <si>
+    <t>US4</t>
+  </si>
+  <si>
+    <t>US5</t>
+  </si>
+  <si>
+    <t>US6</t>
+  </si>
+  <si>
+    <t>US7</t>
+  </si>
+  <si>
+    <t>US8</t>
+  </si>
+  <si>
+    <t>US9</t>
+  </si>
+  <si>
+    <t>US10</t>
+  </si>
+  <si>
+    <t>US11</t>
+  </si>
+  <si>
+    <t>US12</t>
+  </si>
+  <si>
+    <t>US13</t>
+  </si>
+  <si>
+    <t>US14</t>
+  </si>
+  <si>
+    <t>US15</t>
+  </si>
+  <si>
+    <t>US16</t>
+  </si>
+  <si>
+    <t>US17</t>
+  </si>
+  <si>
+    <t>US18</t>
+  </si>
+  <si>
+    <t>US16.1</t>
+  </si>
+  <si>
+    <t>US16.2</t>
+  </si>
+  <si>
+    <t>US19</t>
+  </si>
+  <si>
+    <t>US20</t>
+  </si>
+  <si>
+    <t>US21</t>
+  </si>
+  <si>
+    <t>US22</t>
+  </si>
+  <si>
+    <t>US23</t>
+  </si>
+  <si>
+    <t>US24</t>
+  </si>
+  <si>
+    <t>US25</t>
+  </si>
+  <si>
+    <t>US26</t>
+  </si>
+  <si>
+    <t>US27</t>
+  </si>
+  <si>
+    <t>US28</t>
+  </si>
+  <si>
+    <t>US29</t>
+  </si>
+  <si>
+    <t>US30</t>
+  </si>
+  <si>
+    <t>US31</t>
+  </si>
+  <si>
+    <t>US32</t>
+  </si>
+  <si>
+    <t>US33</t>
+  </si>
+  <si>
+    <t>US34</t>
+  </si>
+  <si>
+    <t>US35</t>
+  </si>
+  <si>
+    <t>Dependencies</t>
+  </si>
+  <si>
+    <t>US20, US21, US22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a marker, I want to receive feedback as confirmation messagesfrom the application for all my interactions so that I know it has been successful. </t>
+  </si>
+  <si>
+    <t>US25, US26</t>
+  </si>
+  <si>
+    <t>US29/US30</t>
   </si>
 </sst>
 </file>
@@ -738,21 +861,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="135.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="135.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -765,25 +888,30 @@
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="B4" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="7">
         <v>3</v>
@@ -792,10 +920,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="B5" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="7">
         <v>3</v>
@@ -804,10 +934,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+    <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="B6" s="8" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C6" s="7">
         <v>2</v>
@@ -816,10 +948,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+    <row r="7" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="B7" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" s="7">
         <v>3</v>
@@ -828,26 +962,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="8"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+    <row r="11" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="B11" s="8" t="s">
         <v>4</v>
       </c>
@@ -858,10 +994,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+    <row r="12" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="B12" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C12" s="7">
         <v>3</v>
@@ -869,11 +1007,16 @@
       <c r="D12" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="B13" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" s="7">
         <v>1</v>
@@ -881,11 +1024,16 @@
       <c r="D13" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="B14" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="7">
         <v>2</v>
@@ -893,9 +1041,14 @@
       <c r="D14" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="B15" s="8" t="s">
         <v>5</v>
       </c>
@@ -905,9 +1058,14 @@
       <c r="D15" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B16" s="8" t="s">
         <v>6</v>
       </c>
@@ -917,9 +1075,14 @@
       <c r="D16" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
+      <c r="E16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="B17" s="8" t="s">
         <v>7</v>
       </c>
@@ -929,9 +1092,14 @@
       <c r="D17" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="B18" s="8" t="s">
         <v>8</v>
       </c>
@@ -941,9 +1109,14 @@
       <c r="D18" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="B19" s="8" t="s">
         <v>9</v>
       </c>
@@ -954,8 +1127,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+    <row r="20" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="B20" s="8" t="s">
         <v>10</v>
       </c>
@@ -965,9 +1140,14 @@
       <c r="D20" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="B21" s="8" t="s">
         <v>11</v>
       </c>
@@ -977,14 +1157,17 @@
       <c r="D21" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
       <c r="B22" s="8"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>12</v>
       </c>
@@ -992,22 +1175,24 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
       <c r="B24" s="8"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
+    <row r="26" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="B26" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C26" s="7">
         <v>4</v>
@@ -1016,32 +1201,38 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
+    <row r="27" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="B27" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
+    <row r="28" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="B28" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
+    <row r="29" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="4"/>
       <c r="B29" s="11"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
+    <row r="30" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="B30" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" s="7">
         <v>3</v>
@@ -1049,9 +1240,14 @@
       <c r="D30" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
+      <c r="E30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B31" s="8" t="s">
         <v>13</v>
       </c>
@@ -1061,11 +1257,16 @@
       <c r="D31" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
+      <c r="E31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="B32" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C32" s="7">
         <v>4</v>
@@ -1073,9 +1274,14 @@
       <c r="D32" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
+      <c r="E32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
@@ -1085,9 +1291,14 @@
       <c r="D33" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
+      <c r="E33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="B34" s="8" t="s">
         <v>15</v>
       </c>
@@ -1097,9 +1308,14 @@
       <c r="D34" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
+      <c r="E34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="B35" s="8" t="s">
         <v>16</v>
       </c>
@@ -1109,9 +1325,14 @@
       <c r="D35" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
+      <c r="E35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="B36" s="8" t="s">
         <v>17</v>
       </c>
@@ -1121,11 +1342,16 @@
       <c r="D36" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
+      <c r="E36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="B37" s="8" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="C37" s="7">
         <v>1</v>
@@ -1133,25 +1359,30 @@
       <c r="D37" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
+    <row r="40" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="B40" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C40" s="7">
         <v>5</v>
@@ -1160,10 +1391,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
+    <row r="41" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="B41" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C41" s="7">
         <v>4</v>
@@ -1172,10 +1405,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
+    <row r="42" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="B42" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C42" s="7">
         <v>3</v>
@@ -1183,11 +1418,16 @@
       <c r="D42" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
+      <c r="E42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="B43" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C43" s="7">
         <v>4</v>
@@ -1196,10 +1436,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
+    <row r="44" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="B44" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C44" s="7">
         <v>3</v>
@@ -1208,10 +1450,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
+    <row r="45" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="B45" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C45" s="7">
         <v>3</v>
@@ -1220,34 +1464,43 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
+    <row r="46" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="B46" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="7">
+        <v>2</v>
+      </c>
+      <c r="D46" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="7">
+        <v>4</v>
+      </c>
+      <c r="D47" s="7">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="C46" s="7">
-        <v>2</v>
-      </c>
-      <c r="D46" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="7">
-        <v>4</v>
-      </c>
-      <c r="D47" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="C48" s="7">
         <v>3</v>
@@ -1256,10 +1509,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
+    <row r="49" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="B49" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C49" s="7">
         <v>2</v>
@@ -1268,10 +1523,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
+    <row r="50" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="B50" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C50" s="7">
         <v>1</v>
@@ -1279,8 +1536,11 @@
       <c r="D50" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some extra sub stories
</commit_message>
<xml_diff>
--- a/DomainsModel/User stories classified.xlsx
+++ b/DomainsModel/User stories classified.xlsx
@@ -29,7 +29,7 @@
     <author>Everybody's</author>
   </authors>
   <commentList>
-    <comment ref="B26" authorId="0" shapeId="0">
+    <comment ref="B30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B30" authorId="0" shapeId="0">
+    <comment ref="B34" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B32" authorId="0" shapeId="0">
+    <comment ref="B36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="94">
   <si>
     <t>User Story</t>
   </si>
@@ -424,21 +424,37 @@
   <si>
     <t>US29/US30</t>
   </si>
+  <si>
+    <t>US8.1</t>
+  </si>
+  <si>
+    <t>US8.2</t>
+  </si>
+  <si>
+    <t>US8.3</t>
+  </si>
+  <si>
+    <t>US8.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Team details should include team name (school)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Team details should include team members</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Team details should include team score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Team details should include number of passes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -513,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -521,30 +537,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="8"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
   </cellXfs>
@@ -861,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -873,138 +886,139 @@
     <col min="2" max="2" width="135.1796875" customWidth="1"/>
     <col min="3" max="3" width="17.1796875" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>3</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>3</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="7">
-        <v>2</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="C6" s="6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>3</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="7">
-        <v>4</v>
-      </c>
-      <c r="D11" s="7">
+      <c r="B11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="6">
+        <v>4</v>
+      </c>
+      <c r="D11" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>3</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>2</v>
       </c>
       <c r="E12" t="s">
@@ -1012,16 +1026,16 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="7">
-        <v>1</v>
-      </c>
-      <c r="D13" s="7">
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6">
         <v>1</v>
       </c>
       <c r="E13" t="s">
@@ -1029,16 +1043,16 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="7">
-        <v>2</v>
-      </c>
-      <c r="D14" s="7">
+      <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="D14" s="6">
         <v>1</v>
       </c>
       <c r="E14" t="s">
@@ -1046,502 +1060,531 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C19" s="6">
         <v>3</v>
       </c>
-      <c r="D15" s="7">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D19" s="6">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+    <row r="20" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="7">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+    <row r="21" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="7">
-        <v>4</v>
-      </c>
-      <c r="D17" s="7">
-        <v>2</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="C21" s="6">
+        <v>4</v>
+      </c>
+      <c r="D21" s="6">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+    <row r="22" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="7">
-        <v>2</v>
-      </c>
-      <c r="D18" s="7">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="C22" s="6">
+        <v>2</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+    <row r="23" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C23" s="6">
         <v>3</v>
       </c>
-      <c r="D19" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+      <c r="D23" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="7">
-        <v>1</v>
-      </c>
-      <c r="D20" s="7">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="C24" s="6">
+        <v>1</v>
+      </c>
+      <c r="D24" s="6">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
+    <row r="25" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="7">
-        <v>1</v>
-      </c>
-      <c r="D21" s="7">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="C25" s="6">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="6"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="9" t="s">
+    <row r="26" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="5"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="6"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="5"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="7">
-        <v>4</v>
-      </c>
-      <c r="D26" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+      <c r="C30" s="6">
+        <v>4</v>
+      </c>
+      <c r="D30" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B31" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="4"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="3"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C34" s="6">
         <v>3</v>
       </c>
-      <c r="D30" s="7">
-        <v>2</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D34" s="6">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="4" t="s">
+    <row r="35" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="7">
-        <v>4</v>
-      </c>
-      <c r="D31" s="7">
-        <v>4</v>
-      </c>
-      <c r="E31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="7">
-        <v>4</v>
-      </c>
-      <c r="D32" s="7">
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="7">
-        <v>4</v>
-      </c>
-      <c r="D33" s="7">
-        <v>2</v>
-      </c>
-      <c r="E33" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="7">
-        <v>3</v>
-      </c>
-      <c r="D34" s="7">
-        <v>4</v>
-      </c>
-      <c r="E34" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="7">
-        <v>4</v>
-      </c>
-      <c r="D35" s="7">
-        <v>2</v>
+      <c r="C35" s="6">
+        <v>4</v>
+      </c>
+      <c r="D35" s="6">
+        <v>4</v>
       </c>
       <c r="E35" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="6">
+        <v>4</v>
+      </c>
+      <c r="D36" s="6">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="6">
+        <v>4</v>
+      </c>
+      <c r="D37" s="6">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="6">
+        <v>3</v>
+      </c>
+      <c r="D38" s="6">
+        <v>4</v>
+      </c>
+      <c r="E38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="6">
+        <v>4</v>
+      </c>
+      <c r="D39" s="6">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="7">
-        <v>2</v>
-      </c>
-      <c r="D36" s="7">
-        <v>1</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="C40" s="6">
+        <v>2</v>
+      </c>
+      <c r="D40" s="6">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="4" t="s">
+    <row r="41" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B41" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C37" s="7">
-        <v>1</v>
-      </c>
-      <c r="D37" s="7">
+      <c r="C41" s="6">
+        <v>1</v>
+      </c>
+      <c r="D41" s="6">
         <v>3</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E41" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-    </row>
-    <row r="39" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="9" t="s">
+    <row r="42" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-    </row>
-    <row r="40" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="4" t="s">
+      <c r="B43" s="5"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B44" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C44" s="6">
         <v>5</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D44" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="4" t="s">
+    <row r="45" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B45" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C41" s="7">
-        <v>4</v>
-      </c>
-      <c r="D41" s="7">
+      <c r="C45" s="6">
+        <v>4</v>
+      </c>
+      <c r="D45" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="4" t="s">
+    <row r="46" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B46" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C46" s="6">
         <v>3</v>
       </c>
-      <c r="D42" s="7">
-        <v>4</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="D46" s="6">
+        <v>4</v>
+      </c>
+      <c r="E46" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
+    <row r="47" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B47" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="7">
-        <v>4</v>
-      </c>
-      <c r="D43" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="4" t="s">
+      <c r="C47" s="6">
+        <v>4</v>
+      </c>
+      <c r="D47" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B48" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C48" s="6">
         <v>3</v>
       </c>
-      <c r="D44" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="4" t="s">
+      <c r="D48" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B49" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C49" s="6">
         <v>3</v>
       </c>
-      <c r="D45" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="4" t="s">
+      <c r="D49" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B50" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="7">
-        <v>2</v>
-      </c>
-      <c r="D46" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="4" t="s">
+      <c r="C50" s="6">
+        <v>2</v>
+      </c>
+      <c r="D50" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B51" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C47" s="7">
-        <v>4</v>
-      </c>
-      <c r="D47" s="7">
-        <v>2</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="C51" s="6">
+        <v>4</v>
+      </c>
+      <c r="D51" s="6">
+        <v>2</v>
+      </c>
+      <c r="E51" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="4" t="s">
+    <row r="52" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B52" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C52" s="6">
         <v>3</v>
       </c>
-      <c r="D48" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="4" t="s">
+      <c r="D52" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B53" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="7">
-        <v>2</v>
-      </c>
-      <c r="D49" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="4" t="s">
+      <c r="C53" s="6">
+        <v>2</v>
+      </c>
+      <c r="D53" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B54" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="7">
-        <v>1</v>
-      </c>
-      <c r="D50" s="7">
-        <v>1</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="C54" s="6">
+        <v>1</v>
+      </c>
+      <c r="D54" s="6">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>